<commit_message>
added more documentation for decision tables in prep for coding
</commit_message>
<xml_diff>
--- a/DecisionTables.xlsx
+++ b/DecisionTables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>DICE ROLL</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>DECISION TABLE FOR JUST ONE PLAYER'S MARBLES ON BOARD (not taking into affect other players playing at the same time)</t>
-  </si>
-  <si>
     <t>2,3,4,5</t>
   </si>
   <si>
@@ -93,6 +90,15 @@
   </si>
   <si>
     <t>move one of four marbles on table dice roll</t>
+  </si>
+  <si>
+    <t>DECISION TABLE FOR JUST ONE PLAYER'S MARBLES ON BOARD (not taking into affect other players playing at the same time) - so start here is only occuppied by one of playerX's 4 marbles, not another player yet…</t>
+  </si>
+  <si>
+    <t>next to take into consideration is other players</t>
+  </si>
+  <si>
+    <t>can we jump ourselves? And what about shortcuts of the corners (i.e. land on an inside corner exactly &amp; next time you roll 3, then can jump corner to corner)?</t>
   </si>
 </sst>
 </file>
@@ -450,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD65E9E-546F-4C97-AC00-4BCB079C2C6F}">
-  <dimension ref="A3:E14"/>
+  <dimension ref="A3:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E11" activeCellId="3" sqref="E6 E8 E10 E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,7 +473,7 @@
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -489,7 +495,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -506,7 +512,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -557,7 +563,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
@@ -566,7 +572,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>13</v>
@@ -574,7 +580,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -583,7 +589,7 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>13</v>
@@ -591,7 +597,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -600,7 +606,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
@@ -608,7 +614,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -617,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
@@ -625,7 +631,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -634,10 +640,20 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>